<commit_message>
test: Add test records to Excel and Open Office test documents
</commit_message>
<xml_diff>
--- a/components/system/src/test-reference/data/org/formulacompiler/tests/reference/FinancialFunctions.xlsx
+++ b/components/system/src/test-reference/data/org/formulacompiler/tests/reference/FinancialFunctions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14460" windowHeight="13905"/>
@@ -32,6 +32,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>peo:</t>
         </r>
@@ -40,6 +42,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -54,6 +58,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>peo:</t>
         </r>
@@ -62,6 +68,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Requires fractional exponents.</t>
@@ -76,6 +84,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -84,6 +94,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -98,6 +110,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -106,6 +120,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -120,6 +136,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -128,6 +146,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -142,6 +162,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -150,6 +172,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -164,6 +188,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -172,6 +198,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -186,6 +214,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -194,6 +224,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -208,6 +240,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -216,6 +250,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -230,6 +266,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -238,6 +276,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -252,6 +292,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -260,6 +302,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -274,6 +318,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -282,6 +328,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -296,6 +344,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -304,6 +354,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -318,6 +370,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -326,6 +380,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -340,6 +396,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -348,6 +406,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -362,6 +422,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -370,6 +432,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -384,6 +448,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -392,6 +458,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -406,6 +474,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -414,6 +484,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -428,6 +500,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -436,6 +510,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -450,6 +526,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -458,6 +536,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -472,6 +552,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -480,6 +562,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -494,6 +578,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -502,6 +588,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -516,6 +604,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -524,6 +614,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -538,6 +630,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -546,6 +640,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -560,6 +656,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>Vladimir Korenev:</t>
         </r>
@@ -568,6 +666,8 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
 Precision problem</t>
@@ -579,7 +679,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Actual</t>
   </si>
@@ -652,11 +752,17 @@
   <si>
     <t>Custom check</t>
   </si>
+  <si>
+    <t>XIRR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -665,11 +771,15 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <i/>
@@ -681,12 +791,16 @@
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
@@ -715,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -726,11 +840,783 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="114">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1050,20 +1936,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q83"/>
+  <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:IV1"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="N88" sqref="N88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="14.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
     <col min="4" max="4" width="9.25" customWidth="1"/>
     <col min="5" max="5" width="10.25" customWidth="1"/>
-    <col min="6" max="9" width="6.125" customWidth="1"/>
+    <col min="6" max="6" width="6.75" customWidth="1"/>
+    <col min="7" max="8" width="6.125" customWidth="1"/>
+    <col min="9" max="9" width="8.5" customWidth="1"/>
     <col min="10" max="10" width="10.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="24.25" customWidth="1"/>
     <col min="14" max="14" width="14.125" bestFit="1" customWidth="1"/>
@@ -3659,24 +4547,779 @@
         <v>1</v>
       </c>
     </row>
+    <row r="85" spans="1:17">
+      <c r="A85">
+        <v>-0.4486799232661724</v>
+      </c>
+      <c r="B85">
+        <f t="shared" ref="B85" si="14">XIRR(F85:H85,C85:E85,I85)</f>
+        <v>-0.4486799232661724</v>
+      </c>
+      <c r="C85" s="8">
+        <v>39448.166666666664</v>
+      </c>
+      <c r="D85" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E85" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F85" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="G85" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H85" s="5">
+        <v>4250</v>
+      </c>
+      <c r="I85" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J85" s="1">
+        <v>7</v>
+      </c>
+      <c r="K85" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L85" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P85" t="b">
+        <f t="shared" ref="P85:P91" si="15">OR(ISBLANK(B85),IF(ISERROR(B85),ERROR.TYPE(B85)=IF(ISBLANK(M85),ERROR.TYPE(A85),ERROR.TYPE(M85)),IF(ISBLANK(M85),AND(NOT(ISBLANK(A85)),A85=B85),B85=M85)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q85" t="b">
+        <f t="shared" ref="Q85:Q91" si="16">IF(ISBLANK(O85),IF(ISERROR(P85),FALSE,P85),O85)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17">
+      <c r="A86">
+        <v>-0.4486799232661724</v>
+      </c>
+      <c r="B86">
+        <f>XIRR(F86:H86,C86:E86)</f>
+        <v>-0.4486799232661724</v>
+      </c>
+      <c r="C86" s="8">
+        <v>39448</v>
+      </c>
+      <c r="D86" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E86" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F86" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="G86" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H86" s="5">
+        <v>4250</v>
+      </c>
+      <c r="J86" s="1">
+        <v>6</v>
+      </c>
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="P86" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q86" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
+      <c r="A87">
+        <v>-0.44867992773652066</v>
+      </c>
+      <c r="B87">
+        <f t="shared" ref="B87:B91" si="17">XIRR(F87:H87,C87:E87,I87)</f>
+        <v>-0.44867992773652066</v>
+      </c>
+      <c r="C87" s="8">
+        <v>39448</v>
+      </c>
+      <c r="D87" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E87" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F87" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="G87" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H87" s="5">
+        <v>4250</v>
+      </c>
+      <c r="I87">
+        <v>-0.7</v>
+      </c>
+      <c r="J87" s="1">
+        <v>7</v>
+      </c>
+      <c r="P87" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q87" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
+      <c r="A88" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" t="e">
+        <f t="shared" si="17"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C88" s="8">
+        <v>39448</v>
+      </c>
+      <c r="D88" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E88" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F88" s="5">
+        <v>10000</v>
+      </c>
+      <c r="G88" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H88" s="5">
+        <v>4250</v>
+      </c>
+      <c r="I88">
+        <v>0.1</v>
+      </c>
+      <c r="J88" s="1">
+        <v>7</v>
+      </c>
+      <c r="K88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P88" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q88" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17">
+      <c r="A89">
+        <v>-0.44867992986716332</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="17"/>
+        <v>-0.44867992986716332</v>
+      </c>
+      <c r="C89" s="8">
+        <v>39448</v>
+      </c>
+      <c r="D89" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E89" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F89" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="G89" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H89" s="5">
+        <v>4250</v>
+      </c>
+      <c r="I89">
+        <v>-0.99999000000000005</v>
+      </c>
+      <c r="J89" s="1">
+        <v>7</v>
+      </c>
+      <c r="P89" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q89" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17">
+      <c r="A90" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" t="e">
+        <f t="shared" si="17"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C90" s="8">
+        <v>39448</v>
+      </c>
+      <c r="D90" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E90" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F90" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="G90" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H90" s="5">
+        <v>4250</v>
+      </c>
+      <c r="I90">
+        <v>-1</v>
+      </c>
+      <c r="J90" s="1">
+        <v>7</v>
+      </c>
+      <c r="M90" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P90" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q90" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
+      <c r="A91" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" t="e">
+        <f t="shared" si="17"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C91" s="8">
+        <v>39448</v>
+      </c>
+      <c r="D91" s="9">
+        <v>39508</v>
+      </c>
+      <c r="E91" s="9">
+        <v>39751</v>
+      </c>
+      <c r="F91" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="G91" s="5">
+        <v>2750</v>
+      </c>
+      <c r="H91" s="5">
+        <v>4250</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91" s="1">
+        <v>7</v>
+      </c>
+      <c r="M91" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P91" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q91" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10000">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="111" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q2),Q2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="112" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M2),ISBLANK(O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I10000">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="113" stopIfTrue="1">
       <formula>$J2&gt;COLUMN(C2)-3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M10000">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="114" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M2)),IF(ISERROR(A2),ERROR.TYPE(A2)=ERROR.TYPE(M2),A2=M2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85:A91">
+    <cfRule type="expression" dxfId="109" priority="109" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q85),Q85))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="110" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M85),ISBLANK(O85)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C85:I91">
+    <cfRule type="expression" dxfId="107" priority="108" stopIfTrue="1">
+      <formula>$J85&gt;COLUMN(C85)-3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M85:M91">
+    <cfRule type="expression" dxfId="106" priority="107" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M85)),IF(ISERROR(A85),ERROR.TYPE(A85)=ERROR.TYPE(M85),A85=M85))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="105" priority="105" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="106" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="103" priority="103" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="102" priority="104" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="101" priority="101" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="102" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="99" priority="99" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="100" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="98" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="95" priority="95" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="94" priority="96" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M87">
+    <cfRule type="expression" dxfId="93" priority="94" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M87)),IF(ISERROR(A87),ERROR.TYPE(A87)=ERROR.TYPE(M87),A87=M87))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="92" priority="92" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="93" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="90" priority="90" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="91" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="88" priority="88" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="89" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="86" priority="86" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="87" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="84" priority="84" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="85" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="82" priority="82" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="83" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M90">
+    <cfRule type="expression" dxfId="80" priority="81" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M90)),IF(ISERROR(A90),ERROR.TYPE(A90)=ERROR.TYPE(M90),A90=M90))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M87">
+    <cfRule type="expression" dxfId="79" priority="80" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M87)),IF(ISERROR(A87),ERROR.TYPE(A87)=ERROR.TYPE(M87),A87=M87))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M90">
+    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M90)),IF(ISERROR(A90),ERROR.TYPE(A90)=ERROR.TYPE(M90),A90=M90))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="77" priority="77" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="78" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="75" priority="75" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="76" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="73" priority="73" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="74" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="71" priority="71" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="72" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="69" priority="69" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="70" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="67" priority="67" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="68" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="65" priority="65" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q88),Q88))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="66" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M88),ISBLANK(O88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="63" priority="63" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q88),Q88))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="64" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M88),ISBLANK(O88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="61" priority="61" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q88),Q88))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="62" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M88),ISBLANK(O88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="59" priority="59" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q88),Q88))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="60" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M88),ISBLANK(O88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="57" priority="57" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q88),Q88))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="58" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M88),ISBLANK(O88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88">
+    <cfRule type="expression" dxfId="55" priority="55" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q88),Q88))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="56" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M88),ISBLANK(O88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M88">
+    <cfRule type="expression" dxfId="53" priority="54" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M88)),IF(ISERROR(A88),ERROR.TYPE(A88)=ERROR.TYPE(M88),A88=M88))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="52" priority="52" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="53" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="50" priority="50" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="51" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="48" priority="48" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="49" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="47" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="expression" dxfId="42" priority="42" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q91),Q91))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="43" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M91),ISBLANK(O91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M91">
+    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M91)),IF(ISERROR(A91),ERROR.TYPE(A91)=ERROR.TYPE(M91),A91=M91))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M88">
+    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M88)),IF(ISERROR(A88),ERROR.TYPE(A88)=ERROR.TYPE(M88),A88=M88))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M91">
+    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M91)),IF(ISERROR(A91),ERROR.TYPE(A91)=ERROR.TYPE(M91),A91=M91))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="37" priority="37" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A87">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q87),Q87))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M87),ISBLANK(O87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A90">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q90),Q90))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M90),ISBLANK(O90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M90">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M90)),IF(ISERROR(A90),ERROR.TYPE(A90)=ERROR.TYPE(M90),A90=M90))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M90">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M90)),IF(ISERROR(A90),ERROR.TYPE(A90)=ERROR.TYPE(M90),A90=M90))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>